<commit_message>
Add system block design
</commit_message>
<xml_diff>
--- a/timing diagram.xlsx
+++ b/timing diagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\intelight\intelight\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03D781C-AD9D-4CCF-ACAB-F30E028C1689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41138989-9462-49D6-AE93-90577A9B31D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{87E2AC90-7B75-480B-AA1B-B9BFC3F20644}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="77">
   <si>
     <t>POLICY GENERATOR</t>
   </si>
@@ -258,6 +258,12 @@
   </si>
   <si>
     <t>new Q 0</t>
+  </si>
+  <si>
+    <t>GSG</t>
+  </si>
+  <si>
+    <t>goal sig</t>
   </si>
 </sst>
 </file>
@@ -412,7 +418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
@@ -423,6 +429,20 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -438,20 +458,8 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,7 +660,7 @@
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>426720</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1115,10 +1123,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="10"/>
+      <c r="B1" s="22"/>
       <c r="C1" t="s">
         <v>39</v>
       </c>
@@ -1151,34 +1159,34 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="10" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1189,7 +1197,7 @@
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1197,7 +1205,7 @@
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="14" t="s">
         <v>50</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -1205,26 +1213,26 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C8" t="str">
@@ -1236,7 +1244,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="15" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1244,12 +1252,12 @@
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="13" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -1264,7 +1272,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="15" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -1278,7 +1286,7 @@
       <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C13" t="str">
@@ -1290,7 +1298,7 @@
       </c>
     </row>
     <row r="14" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -1301,26 +1309,26 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="25"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C16" t="str">
@@ -1332,7 +1340,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="16" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -1346,7 +1354,7 @@
       <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C18" t="str">
@@ -1358,7 +1366,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="16" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="5" t="s">
@@ -1369,7 +1377,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="16" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="5" t="s">
@@ -1383,7 +1391,7 @@
       <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C21" t="str">
@@ -1395,7 +1403,7 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C22" t="str">
@@ -1407,7 +1415,7 @@
       </c>
     </row>
     <row r="23" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="16" t="s">
         <v>20</v>
       </c>
       <c r="C23" s="5" t="s">
@@ -1421,12 +1429,12 @@
       <c r="A24" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="13" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="16" t="s">
         <v>22</v>
       </c>
       <c r="C25" s="5" t="s">
@@ -1440,12 +1448,12 @@
       <c r="A26" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="13" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="16" t="s">
         <v>24</v>
       </c>
       <c r="C27" s="5" t="s">
@@ -1456,26 +1464,26 @@
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="26"/>
+      <c r="K28" s="26"/>
+      <c r="L28" s="26"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>6</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -1487,7 +1495,7 @@
       </c>
     </row>
     <row r="30" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="23" t="s">
+      <c r="B30" s="17" t="s">
         <v>34</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -1501,7 +1509,7 @@
       <c r="A31" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="11" t="s">
         <v>34</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -1512,7 +1520,7 @@
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="11" t="s">
         <v>36</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -1523,7 +1531,7 @@
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="11" t="s">
         <v>32</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -1534,7 +1542,7 @@
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C34" t="s">
@@ -1545,7 +1553,7 @@
       </c>
     </row>
     <row r="35" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="23" t="s">
+      <c r="B35" s="17" t="s">
         <v>26</v>
       </c>
       <c r="C35" s="6" t="s">
@@ -1556,26 +1564,26 @@
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" s="15" t="s">
+      <c r="A36" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="15"/>
-      <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="21"/>
+      <c r="K36" s="21"/>
+      <c r="L36" s="21"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="11" t="s">
         <v>26</v>
       </c>
       <c r="C37" t="s">
@@ -1586,7 +1594,7 @@
       </c>
     </row>
     <row r="38" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="24" t="s">
+      <c r="B38" s="18" t="s">
         <v>27</v>
       </c>
       <c r="C38" s="7" t="s">
@@ -1600,7 +1608,7 @@
       <c r="A39" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="11" t="s">
         <v>28</v>
       </c>
       <c r="C39" s="1" t="s">
@@ -1611,7 +1619,7 @@
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B40" s="17" t="s">
+      <c r="B40" s="11" t="s">
         <v>51</v>
       </c>
       <c r="C40" s="1" t="s">
@@ -1623,7 +1631,7 @@
       </c>
     </row>
     <row r="41" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="24" t="s">
+      <c r="B41" s="18" t="s">
         <v>29</v>
       </c>
       <c r="C41" s="1" t="s">
@@ -1637,12 +1645,12 @@
       <c r="A42" t="s">
         <v>30</v>
       </c>
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="13" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B43" s="25" t="s">
+      <c r="B43" s="19" t="s">
         <v>27</v>
       </c>
       <c r="C43" s="8" t="s">
@@ -1653,7 +1661,7 @@
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B44" s="25" t="s">
+      <c r="B44" s="19" t="s">
         <v>29</v>
       </c>
       <c r="C44" s="1" t="s">
@@ -1664,7 +1672,7 @@
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B45" s="25" t="s">
+      <c r="B45" s="19" t="s">
         <v>24</v>
       </c>
       <c r="C45" s="1" t="s">
@@ -1675,7 +1683,7 @@
       </c>
     </row>
     <row r="46" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="26" t="s">
+      <c r="B46" s="20" t="s">
         <v>32</v>
       </c>
       <c r="C46" s="1" t="s">
@@ -1703,10 +1711,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{128F7C61-DBDE-4795-B53E-7B3365EBC957}">
-  <dimension ref="A1:L46"/>
+  <dimension ref="A1:L48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1717,10 +1725,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="10"/>
+      <c r="B1" s="22"/>
       <c r="C1" t="s">
         <v>39</v>
       </c>
@@ -1753,31 +1761,31 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="12" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1785,7 +1793,7 @@
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1793,34 +1801,34 @@
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="20"/>
+      <c r="C6" s="14"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="15" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1828,17 +1836,17 @@
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="13" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="15" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1846,247 +1854,261 @@
       <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="13" t="s">
+    <row r="15" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="27"/>
+    </row>
+    <row r="16" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="22" t="s">
-        <v>15</v>
-      </c>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="25"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B20" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="22" t="s">
+    <row r="21" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="22" t="s">
+    <row r="22" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B23" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B22" s="17" t="s">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B24" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="9"/>
-    </row>
-    <row r="23" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="22" t="s">
+      <c r="D24" s="9"/>
+    </row>
+    <row r="25" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="16" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" s="19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="22" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="B28" s="13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="22" t="s">
+    <row r="29" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" s="14" t="s">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>6</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="23" t="s">
-        <v>34</v>
-      </c>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
+      <c r="K30" s="26"/>
+      <c r="L30" s="26"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B33" s="11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B32" s="17" t="s">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B34" s="11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B33" s="17" t="s">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B35" s="11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B34" s="17" t="s">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B36" s="11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="15"/>
-      <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>14</v>
-      </c>
+    <row r="37" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B37" s="17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="24" t="s">
-        <v>27</v>
-      </c>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" s="21"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="21"/>
+      <c r="K38" s="21"/>
+      <c r="L38" s="21"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B41" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B40" s="17" t="s">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B42" s="11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="24" t="s">
+    <row r="43" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>30</v>
       </c>
-      <c r="B42" s="19" t="s">
+      <c r="B44" s="13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B43" s="25" t="s">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B45" s="19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B44" s="25" t="s">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B46" s="19" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B45" s="25" t="s">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B47" s="19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="26" t="s">
+    <row r="48" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="20" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A38:L38"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="A7:L7"/>
-    <mergeCell ref="A15:L15"/>
-    <mergeCell ref="A28:L28"/>
-    <mergeCell ref="A36:L36"/>
+    <mergeCell ref="A17:L17"/>
+    <mergeCell ref="A30:L30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Update post sync testbench
</commit_message>
<xml_diff>
--- a/timing diagram.xlsx
+++ b/timing diagram.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\intelight\intelight\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981945B1-3A57-472F-9C9D-6D37649D9AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4703589C-0D6D-4E0C-BFD5-E4247EC3449C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8340" yWindow="3180" windowWidth="17280" windowHeight="8964" activeTab="4" xr2:uid="{87E2AC90-7B75-480B-AA1B-B9BFC3F20644}"/>
+    <workbookView xWindow="-9228" yWindow="3336" windowWidth="17280" windowHeight="8964" activeTab="4" xr2:uid="{87E2AC90-7B75-480B-AA1B-B9BFC3F20644}"/>
   </bookViews>
   <sheets>
     <sheet name="ideal" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1484" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1495" uniqueCount="262">
   <si>
     <t>POLICY GENERATOR</t>
   </si>
@@ -816,6 +816,12 @@
   </si>
   <si>
     <t>goal_sig_4</t>
+  </si>
+  <si>
+    <t>CC0</t>
+  </si>
+  <si>
+    <t>1 register (internal)</t>
   </si>
 </sst>
 </file>
@@ -1091,6 +1097,15 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1101,15 +1116,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5617,10 +5623,10 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="65"/>
+      <c r="B2" s="68"/>
       <c r="C2" s="37" t="s">
         <v>136</v>
       </c>
@@ -5724,10 +5730,10 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="64"/>
+      <c r="B7" s="67"/>
       <c r="C7" s="39" t="s">
         <v>136</v>
       </c>
@@ -5973,10 +5979,10 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="63" t="s">
+      <c r="A17" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="63"/>
+      <c r="B17" s="66"/>
       <c r="C17" s="36"/>
       <c r="D17" s="36" t="s">
         <v>136</v>
@@ -6329,10 +6335,10 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A30" s="62" t="s">
+      <c r="A30" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="62"/>
+      <c r="B30" s="65"/>
       <c r="C30" s="35" t="s">
         <v>138</v>
       </c>
@@ -6381,11 +6387,11 @@
       <c r="B32" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C32" s="66" t="s">
+      <c r="C32" s="62" t="s">
         <v>130</v>
       </c>
-      <c r="D32" s="67"/>
-      <c r="E32" s="67"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="63"/>
       <c r="F32" s="2" t="s">
         <v>87</v>
       </c>
@@ -6502,11 +6508,11 @@
       <c r="B36" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="66" t="s">
+      <c r="C36" s="62" t="s">
         <v>130</v>
       </c>
-      <c r="D36" s="67"/>
-      <c r="E36" s="67"/>
+      <c r="D36" s="63"/>
+      <c r="E36" s="63"/>
       <c r="F36" s="2" t="s">
         <v>53</v>
       </c>
@@ -6588,10 +6594,10 @@
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A39" s="68" t="s">
+      <c r="A39" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="B39" s="68"/>
+      <c r="B39" s="64"/>
       <c r="C39" s="38"/>
       <c r="D39" s="38"/>
       <c r="E39" s="38"/>
@@ -6699,11 +6705,11 @@
       <c r="B43" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C43" s="66" t="s">
+      <c r="C43" s="62" t="s">
         <v>130</v>
       </c>
-      <c r="D43" s="67"/>
-      <c r="E43" s="67"/>
+      <c r="D43" s="63"/>
+      <c r="E43" s="63"/>
       <c r="F43" t="s">
         <v>50</v>
       </c>
@@ -6848,10 +6854,10 @@
       <c r="C48" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="D48" s="67" t="s">
+      <c r="D48" s="63" t="s">
         <v>132</v>
       </c>
-      <c r="E48" s="67"/>
+      <c r="E48" s="63"/>
       <c r="F48" t="s">
         <v>86</v>
       </c>
@@ -6902,16 +6908,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A1:B1"/>
     <mergeCell ref="C32:E32"/>
     <mergeCell ref="C36:E36"/>
     <mergeCell ref="C43:E43"/>
     <mergeCell ref="D48:E48"/>
     <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6922,10 +6928,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81B2956E-40A3-4431-A583-0A8164570B28}">
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="83" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6965,68 +6971,76 @@
         <v>248</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="47" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="70" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="69" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="69"/>
+      <c r="C2" t="s">
+        <v>260</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="70" t="s">
         <v>181</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="F2" s="54" t="s">
+      <c r="B3" s="70"/>
+      <c r="F3" s="54" t="s">
         <v>136</v>
       </c>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="27" t="s">
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="27" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="71" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="71" t="s">
         <v>139</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>151</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D3" s="48" t="s">
+      <c r="D4" s="48" t="s">
         <v>157</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E4" s="42" t="s">
         <v>195</v>
       </c>
-      <c r="F3" s="51" t="s">
+      <c r="F4" s="51" t="s">
         <v>193</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>224</v>
-      </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="71"/>
-      <c r="B4" t="s">
-        <v>152</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D4" s="48" t="s">
-        <v>158</v>
-      </c>
-      <c r="E4" s="42" t="s">
-        <v>194</v>
-      </c>
-      <c r="F4" s="51" t="s">
-        <v>212</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>225</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
@@ -7034,11 +7048,9 @@
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="71" t="s">
-        <v>140</v>
-      </c>
+      <c r="A5" s="71"/>
       <c r="B5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>143</v>
@@ -7061,220 +7073,221 @@
       <c r="K5" s="9"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="71"/>
+      <c r="A6" s="71" t="s">
+        <v>140</v>
+      </c>
       <c r="B6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D6" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="E6" s="42" t="s">
+        <v>194</v>
+      </c>
+      <c r="F6" s="51" t="s">
+        <v>212</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="71"/>
+      <c r="B7" t="s">
         <v>154</v>
-      </c>
-      <c r="C6" s="33" t="s">
-        <v>185</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E6" s="48" t="s">
-        <v>159</v>
-      </c>
-      <c r="F6" s="42" t="s">
-        <v>196</v>
-      </c>
-      <c r="G6" s="51" t="s">
-        <v>211</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="71" t="s">
-        <v>141</v>
-      </c>
-      <c r="B7" t="s">
-        <v>155</v>
       </c>
       <c r="C7" s="33" t="s">
         <v>185</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E7" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="F7" s="42" t="s">
+        <v>196</v>
+      </c>
+      <c r="G7" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="71" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E7" s="48" t="s">
+      <c r="E8" s="48" t="s">
         <v>158</v>
       </c>
-      <c r="F7" s="42" t="s">
+      <c r="F8" s="42" t="s">
         <v>194</v>
       </c>
-      <c r="G7" s="51" t="s">
+      <c r="G8" s="51" t="s">
         <v>212</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>225</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="71"/>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E8" s="48" t="s">
-        <v>168</v>
-      </c>
-      <c r="F8" s="42" t="s">
-        <v>201</v>
-      </c>
-      <c r="G8" s="51" t="s">
-        <v>210</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="71"/>
       <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E9" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="F9" s="42" t="s">
+        <v>201</v>
+      </c>
+      <c r="G9" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="71"/>
+      <c r="B10" t="s">
         <v>156</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D10" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F9" s="48" t="s">
+      <c r="F10" s="48" t="s">
         <v>197</v>
       </c>
-      <c r="G9" s="42" t="s">
+      <c r="G10" s="42" t="s">
         <v>208</v>
       </c>
-      <c r="H9" s="51" t="s">
+      <c r="H10" s="51" t="s">
         <v>213</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I10" s="4" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>30</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>147</v>
       </c>
-      <c r="C10" s="45"/>
-      <c r="E10" s="48" t="s">
+      <c r="C11" s="45"/>
+      <c r="E11" s="48" t="s">
         <v>159</v>
       </c>
-      <c r="F10" s="42" t="s">
+      <c r="F11" s="42" t="s">
         <v>196</v>
       </c>
-      <c r="G10" s="51" t="s">
+      <c r="G11" s="51" t="s">
         <v>211</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>227</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>148</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="F11" s="48" t="s">
-        <v>197</v>
-      </c>
-      <c r="G11" s="42" t="s">
-        <v>208</v>
-      </c>
-      <c r="H11" s="51" t="s">
-        <v>213</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>60</v>
+        <v>146</v>
       </c>
       <c r="F12" s="48" t="s">
-        <v>68</v>
+        <v>197</v>
       </c>
       <c r="G12" s="42" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H12" s="51" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
+        <v>149</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="42" t="s">
+        <v>207</v>
+      </c>
+      <c r="H13" s="51" t="s">
+        <v>214</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
         <v>150</v>
-      </c>
-      <c r="E13" s="33" t="s">
-        <v>185</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="G13" s="48" t="s">
-        <v>198</v>
-      </c>
-      <c r="H13" s="50" t="s">
-        <v>209</v>
-      </c>
-      <c r="I13" s="52" t="s">
-        <v>215</v>
-      </c>
-      <c r="J13" s="53" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>139</v>
-      </c>
-      <c r="B14" t="s">
-        <v>161</v>
-      </c>
-      <c r="C14" s="33" t="s">
-        <v>185</v>
-      </c>
-      <c r="D14" s="33" t="s">
-        <v>185</v>
       </c>
       <c r="E14" s="33" t="s">
         <v>185</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="G14" s="49" t="s">
-        <v>157</v>
+        <v>160</v>
+      </c>
+      <c r="G14" s="48" t="s">
+        <v>198</v>
       </c>
       <c r="H14" s="50" t="s">
-        <v>195</v>
-      </c>
-      <c r="I14" s="51" t="s">
-        <v>193</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>224</v>
+        <v>209</v>
+      </c>
+      <c r="I14" s="52" t="s">
+        <v>215</v>
+      </c>
+      <c r="J14" s="53" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>139</v>
+      </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>161</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>185</v>
       </c>
       <c r="D15" s="33" t="s">
         <v>185</v>
@@ -7283,84 +7296,90 @@
         <v>185</v>
       </c>
       <c r="F15" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G15" s="49" t="s">
+        <v>157</v>
+      </c>
+      <c r="H15" s="50" t="s">
+        <v>195</v>
+      </c>
+      <c r="I15" s="51" t="s">
+        <v>193</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="E16" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="G15" s="49" t="s">
+      <c r="G16" s="49" t="s">
         <v>250</v>
       </c>
-      <c r="H15" s="50" t="s">
+      <c r="H16" s="50" t="s">
         <v>251</v>
       </c>
-      <c r="I15" s="51" t="s">
+      <c r="I16" s="51" t="s">
         <v>252</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="J16" s="4" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="70" t="s">
+    <row r="17" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="70" t="s">
         <v>182</v>
       </c>
-      <c r="B16" s="70"/>
-      <c r="C16" s="54" t="s">
+      <c r="B17" s="70"/>
+      <c r="C17" s="54" t="s">
         <v>136</v>
       </c>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="27" t="s">
+      <c r="D17" s="55"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="55"/>
+      <c r="G17" s="55"/>
+      <c r="H17" s="27" t="s">
         <v>239</v>
       </c>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>6</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="E17" s="48" t="s">
+      <c r="E18" s="48" t="s">
         <v>168</v>
       </c>
-      <c r="F17" s="42" t="s">
+      <c r="F18" s="42" t="s">
         <v>201</v>
       </c>
-      <c r="G17" s="51" t="s">
+      <c r="G18" s="51" t="s">
         <v>210</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H18" s="4" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>162</v>
-      </c>
-      <c r="D18" s="48" t="s">
-        <v>167</v>
-      </c>
-      <c r="E18" s="42" t="s">
-        <v>191</v>
-      </c>
-      <c r="F18" s="51" t="s">
-        <v>216</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>231</v>
-      </c>
-    </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>8</v>
-      </c>
       <c r="B19" t="s">
         <v>162</v>
       </c>
@@ -7378,49 +7397,49 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
       <c r="B20" t="s">
-        <v>163</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E20" s="48" t="s">
-        <v>166</v>
-      </c>
-      <c r="F20" s="42" t="s">
-        <v>192</v>
-      </c>
-      <c r="G20" s="51" t="s">
-        <v>217</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>232</v>
+        <v>162</v>
+      </c>
+      <c r="D20" s="48" t="s">
+        <v>167</v>
+      </c>
+      <c r="E20" s="42" t="s">
+        <v>191</v>
+      </c>
+      <c r="F20" s="51" t="s">
+        <v>216</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>164</v>
-      </c>
-      <c r="C21" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="D21" s="48" t="s">
+      <c r="E21" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="E21" s="42" t="s">
+      <c r="F21" s="42" t="s">
         <v>192</v>
       </c>
-      <c r="F21" s="51" t="s">
+      <c r="G21" s="51" t="s">
         <v>217</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="H21" s="4" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>11</v>
-      </c>
       <c r="B22" t="s">
         <v>164</v>
       </c>
@@ -7441,386 +7460,410 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
       <c r="B23" t="s">
+        <v>164</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D23" s="48" t="s">
+        <v>166</v>
+      </c>
+      <c r="E23" s="42" t="s">
+        <v>192</v>
+      </c>
+      <c r="F23" s="51" t="s">
+        <v>217</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D23" s="48" t="s">
+      <c r="D24" s="48" t="s">
         <v>157</v>
       </c>
-      <c r="E23" s="42" t="s">
+      <c r="E24" s="42" t="s">
         <v>195</v>
       </c>
-      <c r="F23" s="51" t="s">
+      <c r="F24" s="51" t="s">
         <v>193</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G24" s="4" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>75</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>254</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="D24" s="48" t="s">
+      <c r="D25" s="48" t="s">
         <v>256</v>
       </c>
-      <c r="E24" s="42" t="s">
+      <c r="E25" s="42" t="s">
         <v>257</v>
       </c>
-      <c r="F24" s="51" t="s">
+      <c r="F25" s="51" t="s">
         <v>258</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="G25" s="4" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="70" t="s">
+    <row r="26" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="70" t="s">
         <v>183</v>
       </c>
-      <c r="B25" s="70"/>
-      <c r="C25" s="47"/>
-      <c r="E25" s="54" t="s">
+      <c r="B26" s="70"/>
+      <c r="C26" s="47"/>
+      <c r="E26" s="54" t="s">
         <v>136</v>
       </c>
-      <c r="F25" s="55"/>
-      <c r="G25" s="55"/>
-      <c r="H25" s="55"/>
-      <c r="I25" s="55"/>
-      <c r="J25" s="27" t="s">
+      <c r="F26" s="55"/>
+      <c r="G26" s="55"/>
+      <c r="H26" s="55"/>
+      <c r="I26" s="55"/>
+      <c r="J26" s="27" t="s">
         <v>239</v>
       </c>
-      <c r="K25" s="23"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="K26" s="23"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>140</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D26" s="48" t="s">
+      <c r="D27" s="48" t="s">
         <v>157</v>
       </c>
-      <c r="E26" s="42" t="s">
+      <c r="E27" s="42" t="s">
         <v>195</v>
       </c>
-      <c r="F26" s="51" t="s">
+      <c r="F27" s="51" t="s">
         <v>193</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="G27" s="4" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
         <v>154</v>
       </c>
-      <c r="C27" s="33" t="s">
+      <c r="C28" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="E27" s="48" t="s">
+      <c r="E28" s="48" t="s">
         <v>186</v>
       </c>
-      <c r="F27" s="42" t="s">
+      <c r="F28" s="42" t="s">
         <v>203</v>
       </c>
-      <c r="G27" s="51" t="s">
+      <c r="G28" s="51" t="s">
         <v>218</v>
       </c>
-      <c r="H27" s="4" t="s">
+      <c r="H28" s="4" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>169</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D28" s="48" t="s">
+      <c r="D29" s="48" t="s">
         <v>157</v>
       </c>
-      <c r="E28" s="42" t="s">
+      <c r="E29" s="42" t="s">
         <v>193</v>
       </c>
-      <c r="F28" s="51" t="s">
+      <c r="F29" s="51" t="s">
         <v>193</v>
       </c>
-      <c r="G28" s="4" t="s">
+      <c r="G29" s="4" t="s">
         <v>224</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
-        <v>170</v>
-      </c>
-      <c r="C29" s="33" t="s">
-        <v>185</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="E29" s="48" t="s">
-        <v>187</v>
-      </c>
-      <c r="F29" s="42" t="s">
-        <v>204</v>
-      </c>
-      <c r="G29" s="51" t="s">
-        <v>219</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C30" s="33" t="s">
         <v>185</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E30" s="48" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F30" s="42" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G30" s="51" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>141</v>
-      </c>
       <c r="B31" t="s">
-        <v>12</v>
+        <v>171</v>
       </c>
       <c r="C31" s="33" t="s">
         <v>185</v>
       </c>
       <c r="D31" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E31" s="48" t="s">
+        <v>188</v>
+      </c>
+      <c r="F31" s="42" t="s">
+        <v>205</v>
+      </c>
+      <c r="G31" s="51" t="s">
+        <v>220</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>141</v>
+      </c>
+      <c r="B32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="E31" s="48" t="s">
+      <c r="E32" s="48" t="s">
         <v>157</v>
       </c>
-      <c r="F31" s="42" t="s">
+      <c r="F32" s="42" t="s">
         <v>193</v>
       </c>
-      <c r="G31" s="51" t="s">
+      <c r="G32" s="51" t="s">
         <v>193</v>
       </c>
-      <c r="H31" s="4" t="s">
+      <c r="H32" s="4" t="s">
         <v>224</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B32" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32" s="31"/>
-      <c r="D32" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E32" s="48" t="s">
-        <v>168</v>
-      </c>
-      <c r="F32" s="42" t="s">
-        <v>201</v>
-      </c>
-      <c r="G32" s="51" t="s">
-        <v>210</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="31"/>
+      <c r="D33" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E33" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="F33" s="42" t="s">
+        <v>201</v>
+      </c>
+      <c r="G33" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
         <v>156</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="E33" s="48" t="s">
+      <c r="E34" s="48" t="s">
         <v>189</v>
       </c>
-      <c r="F33" s="42" t="s">
+      <c r="F34" s="42" t="s">
         <v>202</v>
       </c>
-      <c r="G33" s="51" t="s">
+      <c r="G34" s="51" t="s">
         <v>221</v>
       </c>
-      <c r="H33" s="4" t="s">
+      <c r="H34" s="4" t="s">
         <v>234</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>175</v>
-      </c>
-      <c r="D34" s="33" t="s">
-        <v>185</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="F34" s="48" t="s">
-        <v>190</v>
-      </c>
-      <c r="G34" s="42" t="s">
-        <v>206</v>
-      </c>
-      <c r="H34" s="51" t="s">
-        <v>222</v>
-      </c>
-      <c r="I34" s="4" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>175</v>
+      </c>
+      <c r="D35" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="F35" s="48" t="s">
+        <v>190</v>
+      </c>
+      <c r="G35" s="42" t="s">
+        <v>206</v>
+      </c>
+      <c r="H35" s="51" t="s">
+        <v>222</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>141</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F35" s="48" t="s">
+      <c r="F36" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="G35" s="42" t="s">
+      <c r="G36" s="42" t="s">
         <v>207</v>
       </c>
-      <c r="H35" s="51" t="s">
+      <c r="H36" s="51" t="s">
         <v>214</v>
       </c>
-      <c r="I35" s="4" t="s">
+      <c r="I36" s="4" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="36" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="70" t="s">
+    <row r="37" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="70" t="s">
         <v>184</v>
       </c>
-      <c r="B36" s="70"/>
-      <c r="D36" s="54" t="s">
+      <c r="B37" s="70"/>
+      <c r="D37" s="54" t="s">
         <v>136</v>
       </c>
-      <c r="E36" s="55"/>
-      <c r="F36" s="55"/>
-      <c r="G36" s="55"/>
-      <c r="H36" s="55"/>
-      <c r="I36" s="27" t="s">
+      <c r="E37" s="55"/>
+      <c r="F37" s="55"/>
+      <c r="G37" s="55"/>
+      <c r="H37" s="55"/>
+      <c r="I37" s="27" t="s">
         <v>239</v>
       </c>
-      <c r="J36" s="23"/>
-      <c r="K36" s="23"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="J37" s="23"/>
+      <c r="K37" s="23"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>1</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>178</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D37" s="48" t="s">
+      <c r="D38" s="48" t="s">
         <v>158</v>
       </c>
-      <c r="E37" s="42" t="s">
+      <c r="E38" s="42" t="s">
         <v>194</v>
       </c>
-      <c r="F37" s="51" t="s">
+      <c r="F38" s="51" t="s">
         <v>212</v>
       </c>
-      <c r="G37" s="4" t="s">
+      <c r="G38" s="4" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B38" t="s">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
         <v>179</v>
       </c>
-      <c r="C38" s="33" t="s">
+      <c r="C39" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E38" s="48" t="s">
+      <c r="E39" s="48" t="s">
         <v>199</v>
       </c>
-      <c r="F38" s="42" t="s">
+      <c r="F39" s="42" t="s">
         <v>200</v>
       </c>
-      <c r="G38" s="51" t="s">
+      <c r="G39" s="51" t="s">
         <v>223</v>
       </c>
-      <c r="H38" s="4" t="s">
+      <c r="H39" s="4" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>3</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="E39" s="48" t="s">
+      <c r="E40" s="48" t="s">
         <v>168</v>
       </c>
-      <c r="F39" s="42" t="s">
+      <c r="F40" s="42" t="s">
         <v>201</v>
       </c>
-      <c r="G39" s="51" t="s">
+      <c r="G40" s="51" t="s">
         <v>210</v>
       </c>
-      <c r="H39" s="4" t="s">
+      <c r="H40" s="4" t="s">
         <v>226</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A26:B26"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A25:B25"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>